<commit_message>
Realizado Lista e finalizado com Exercicio 5 || Treinado laços de repetição
</commit_message>
<xml_diff>
--- a/Exercicios Laços De Repetição.xlsx
+++ b/Exercicios Laços De Repetição.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Python\Exercícios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03918022-55C7-4BE4-9157-A44A550F1375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA48A1B-A442-4976-9EFA-DE9611F79911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>